<commit_message>
Added IPL EDA in Python_EDA| Modified Car_Dashboard
</commit_message>
<xml_diff>
--- a/EDA_Projects/Dashboards_Excel/Cars_Dashboard.xlsx
+++ b/EDA_Projects/Dashboards_Excel/Cars_Dashboard.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
   <workbookPr hidePivotFieldList="1" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\DataScience\Data_Science_101\EDA_Projects\Dashboards_Excel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\DataScience\Github\Data_Science_101\EDA_Projects\Dashboards_Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{D808A522-DDF7-4A84-BF56-F7E5E864DAA0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80852F26-7F51-4EB6-B57B-86239F090ACA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="330" windowWidth="20730" windowHeight="11310" activeTab="2"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Cars" sheetId="2" r:id="rId1"/>
@@ -21,9 +21,9 @@
     <definedName name="ExternalData_1" localSheetId="0" hidden="1">'Cars'!$A$1:$I$407</definedName>
     <definedName name="Slicer_Origin">#N/A</definedName>
   </definedNames>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
   <pivotCaches>
-    <pivotCache cacheId="6" r:id="rId4"/>
+    <pivotCache cacheId="0" r:id="rId4"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{BBE1A952-AA13-448e-AADC-164F8A28A991}">
@@ -34,20 +34,29 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr/>
     </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/connections.xml><?xml version="1.0" encoding="utf-8"?>
-<connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <connection id="1" keepAlive="1" name="Query - Cars" description="Connection to the 'Cars' query in the workbook." type="5" refreshedVersion="7" background="1" saveData="1">
+<connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16">
+  <connection id="1" xr16:uid="{00000000-0015-0000-FFFF-FFFF00000000}" keepAlive="1" name="Query - Cars" description="Connection to the 'Cars' query in the workbook." type="5" refreshedVersion="7" background="1" saveData="1">
     <dbPr connection="Provider=Microsoft.Mashup.OleDb.1;Data Source=$Workbook$;Location=Cars;Extended Properties=&quot;&quot;" command="SELECT * FROM [Cars]"/>
   </connection>
 </connections>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="857" uniqueCount="332">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="849" uniqueCount="332">
   <si>
     <t>Car</t>
   </si>
@@ -1048,7 +1057,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="21" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1647,6 +1656,29 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="16" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="16" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="20" fillId="34" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="34" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="34" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="34" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="34" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="34" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="18" fillId="33" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1665,30 +1697,7 @@
     <xf numFmtId="0" fontId="19" fillId="33" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="34" borderId="16" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="20" fillId="34" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="34" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="34" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="34" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="34" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="34" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="18" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1891,49 +1900,7 @@
           </a:effectLst>
         </c:spPr>
         <c:marker>
-          <c:symbol val="circle"/>
-          <c:size val="6"/>
-          <c:spPr>
-            <a:gradFill rotWithShape="1">
-              <a:gsLst>
-                <a:gs pos="0">
-                  <a:schemeClr val="accent1">
-                    <a:satMod val="103000"/>
-                    <a:lumMod val="102000"/>
-                    <a:tint val="94000"/>
-                  </a:schemeClr>
-                </a:gs>
-                <a:gs pos="50000">
-                  <a:schemeClr val="accent1">
-                    <a:satMod val="110000"/>
-                    <a:lumMod val="100000"/>
-                    <a:shade val="100000"/>
-                  </a:schemeClr>
-                </a:gs>
-                <a:gs pos="100000">
-                  <a:schemeClr val="accent1">
-                    <a:lumMod val="99000"/>
-                    <a:satMod val="120000"/>
-                    <a:shade val="78000"/>
-                  </a:schemeClr>
-                </a:gs>
-              </a:gsLst>
-              <a:lin ang="5400000" scaled="0"/>
-            </a:gradFill>
-            <a:ln w="9525">
-              <a:solidFill>
-                <a:schemeClr val="accent1"/>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst>
-              <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
-                <a:srgbClr val="000000">
-                  <a:alpha val="63000"/>
-                </a:srgbClr>
-              </a:outerShdw>
-            </a:effectLst>
-          </c:spPr>
+          <c:symbol val="none"/>
         </c:marker>
         <c:dLbl>
           <c:idx val="0"/>
@@ -2124,43 +2091,43 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="13"/>
                 <c:pt idx="0">
-                  <c:v>35</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>29</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>28</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>40</c:v>
+                  <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>27</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>30</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>34</c:v>
+                  <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>28</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>36</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>29</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>29</c:v>
+                  <c:v>9</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>30</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>31</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2505,49 +2472,7 @@
           </a:effectLst>
         </c:spPr>
         <c:marker>
-          <c:symbol val="diamond"/>
-          <c:size val="5"/>
-          <c:spPr>
-            <a:gradFill rotWithShape="1">
-              <a:gsLst>
-                <a:gs pos="0">
-                  <a:schemeClr val="accent1">
-                    <a:satMod val="103000"/>
-                    <a:lumMod val="102000"/>
-                    <a:tint val="94000"/>
-                  </a:schemeClr>
-                </a:gs>
-                <a:gs pos="50000">
-                  <a:schemeClr val="accent1">
-                    <a:satMod val="110000"/>
-                    <a:lumMod val="100000"/>
-                    <a:shade val="100000"/>
-                  </a:schemeClr>
-                </a:gs>
-                <a:gs pos="100000">
-                  <a:schemeClr val="accent1">
-                    <a:lumMod val="99000"/>
-                    <a:satMod val="120000"/>
-                    <a:shade val="78000"/>
-                  </a:schemeClr>
-                </a:gs>
-              </a:gsLst>
-              <a:lin ang="5400000" scaled="0"/>
-            </a:gradFill>
-            <a:ln w="9525">
-              <a:solidFill>
-                <a:schemeClr val="accent1"/>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst>
-              <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
-                <a:srgbClr val="000000">
-                  <a:alpha val="63000"/>
-                </a:srgbClr>
-              </a:outerShdw>
-            </a:effectLst>
-          </c:spPr>
+          <c:symbol val="none"/>
         </c:marker>
         <c:dLbl>
           <c:idx val="0"/>
@@ -3043,8 +2968,7 @@
           </a:effectLst>
         </c:spPr>
         <c:marker>
-          <c:symbol val="circle"/>
-          <c:size val="6"/>
+          <c:symbol val="none"/>
         </c:marker>
         <c:dLbl>
           <c:idx val="0"/>
@@ -3242,56 +3166,6 @@
                 <a:gsLst>
                   <a:gs pos="0">
                     <a:schemeClr val="accent5">
-                      <a:shade val="65000"/>
-                      <a:satMod val="103000"/>
-                      <a:lumMod val="102000"/>
-                      <a:tint val="94000"/>
-                    </a:schemeClr>
-                  </a:gs>
-                  <a:gs pos="50000">
-                    <a:schemeClr val="accent5">
-                      <a:shade val="65000"/>
-                      <a:satMod val="110000"/>
-                      <a:lumMod val="100000"/>
-                      <a:shade val="100000"/>
-                    </a:schemeClr>
-                  </a:gs>
-                  <a:gs pos="100000">
-                    <a:schemeClr val="accent5">
-                      <a:shade val="65000"/>
-                      <a:lumMod val="99000"/>
-                      <a:satMod val="120000"/>
-                      <a:shade val="78000"/>
-                    </a:schemeClr>
-                  </a:gs>
-                </a:gsLst>
-                <a:lin ang="5400000" scaled="0"/>
-              </a:gradFill>
-              <a:ln>
-                <a:noFill/>
-              </a:ln>
-              <a:effectLst>
-                <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
-                  <a:srgbClr val="000000">
-                    <a:alpha val="63000"/>
-                  </a:srgbClr>
-                </a:outerShdw>
-              </a:effectLst>
-            </c:spPr>
-            <c:extLst>
-              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                <c16:uniqueId val="{00000001-DFFA-48D0-BDB6-65077CFCB927}"/>
-              </c:ext>
-            </c:extLst>
-          </c:dPt>
-          <c:dPt>
-            <c:idx val="1"/>
-            <c:bubble3D val="0"/>
-            <c:spPr>
-              <a:gradFill rotWithShape="1">
-                <a:gsLst>
-                  <a:gs pos="0">
-                    <a:schemeClr val="accent5">
                       <a:satMod val="103000"/>
                       <a:lumMod val="102000"/>
                       <a:tint val="94000"/>
@@ -3327,6 +3201,56 @@
             </c:spPr>
             <c:extLst>
               <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000001-DFFA-48D0-BDB6-65077CFCB927}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="1"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:gradFill rotWithShape="1">
+                <a:gsLst>
+                  <a:gs pos="0">
+                    <a:schemeClr val="accent5">
+                      <a:tint val="30000"/>
+                      <a:satMod val="103000"/>
+                      <a:lumMod val="102000"/>
+                      <a:tint val="94000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="50000">
+                    <a:schemeClr val="accent5">
+                      <a:tint val="30000"/>
+                      <a:satMod val="110000"/>
+                      <a:lumMod val="100000"/>
+                      <a:shade val="100000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="100000">
+                    <a:schemeClr val="accent5">
+                      <a:tint val="30000"/>
+                      <a:lumMod val="99000"/>
+                      <a:satMod val="120000"/>
+                      <a:shade val="78000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                </a:gsLst>
+                <a:lin ang="5400000" scaled="0"/>
+              </a:gradFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst>
+                <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+                  <a:srgbClr val="000000">
+                    <a:alpha val="63000"/>
+                  </a:srgbClr>
+                </a:outerShdw>
+              </a:effectLst>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                 <c16:uniqueId val="{00000003-DFFA-48D0-BDB6-65077CFCB927}"/>
               </c:ext>
             </c:extLst>
@@ -3339,7 +3263,7 @@
                 <a:gsLst>
                   <a:gs pos="0">
                     <a:schemeClr val="accent5">
-                      <a:tint val="65000"/>
+                      <a:tint val="60000"/>
                       <a:satMod val="103000"/>
                       <a:lumMod val="102000"/>
                       <a:tint val="94000"/>
@@ -3347,7 +3271,7 @@
                   </a:gs>
                   <a:gs pos="50000">
                     <a:schemeClr val="accent5">
-                      <a:tint val="65000"/>
+                      <a:tint val="60000"/>
                       <a:satMod val="110000"/>
                       <a:lumMod val="100000"/>
                       <a:shade val="100000"/>
@@ -3355,7 +3279,7 @@
                   </a:gs>
                   <a:gs pos="100000">
                     <a:schemeClr val="accent5">
-                      <a:tint val="65000"/>
+                      <a:tint val="60000"/>
                       <a:lumMod val="99000"/>
                       <a:satMod val="120000"/>
                       <a:shade val="78000"/>
@@ -3436,35 +3360,23 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>Calculations!$K$4:$K$6</c:f>
+              <c:f>Calculations!$K$4</c:f>
               <c:strCache>
-                <c:ptCount val="3"/>
+                <c:ptCount val="1"/>
                 <c:pt idx="0">
                   <c:v>Europe</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>Japan</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>US</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Calculations!$L$4:$L$6</c:f>
+              <c:f>Calculations!$L$4</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="3"/>
+                <c:ptCount val="1"/>
                 <c:pt idx="0">
                   <c:v>267.45205479452056</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>304.50632911392404</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>196.88188976377953</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -5200,8 +5112,8 @@
       <xdr:row>2</xdr:row>
       <xdr:rowOff>43640</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:graphicFrame macro="">
           <xdr:nvGraphicFramePr>
             <xdr:cNvPr id="3" name="Origin">
@@ -5226,7 +5138,7 @@
           </a:graphic>
         </xdr:graphicFrame>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="0" name=""/>
@@ -5400,7 +5312,7 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1" refreshedBy="sahil tomar" refreshedDate="44778.709586805555" createdVersion="7" refreshedVersion="7" minRefreshableVersion="3" recordCount="406">
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshedBy="sahil tomar" refreshedDate="44778.709586805555" createdVersion="7" refreshedVersion="7" minRefreshableVersion="3" recordCount="406" xr:uid="{00000000-000A-0000-FFFF-FFFF06000000}">
   <cacheSource type="worksheet">
     <worksheetSource name="Cars"/>
   </cacheSource>
@@ -9931,424 +9843,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable7" cacheId="6" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="7" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="7" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="9" rowHeaderCaption="Region">
-  <location ref="A21:B25" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
-  <pivotFields count="9">
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField dataField="1" showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0">
-      <items count="14">
-        <item x="0"/>
-        <item x="1"/>
-        <item x="2"/>
-        <item x="3"/>
-        <item x="4"/>
-        <item x="5"/>
-        <item x="6"/>
-        <item x="7"/>
-        <item x="8"/>
-        <item x="9"/>
-        <item x="10"/>
-        <item x="11"/>
-        <item x="12"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField axis="axisRow" showAll="0">
-      <items count="4">
-        <item sd="0" x="1"/>
-        <item sd="0" x="2"/>
-        <item sd="0" x="0"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-  </pivotFields>
-  <rowFields count="1">
-    <field x="8"/>
-  </rowFields>
-  <rowItems count="4">
-    <i>
-      <x/>
-    </i>
-    <i>
-      <x v="1"/>
-    </i>
-    <i>
-      <x v="2"/>
-    </i>
-    <i t="grand">
-      <x/>
-    </i>
-  </rowItems>
-  <colItems count="1">
-    <i/>
-  </colItems>
-  <dataFields count="1">
-    <dataField name="Average of Horsepower" fld="4" subtotal="average" baseField="8" baseItem="0"/>
-  </dataFields>
-  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
-      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
-    </ext>
-    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
-      <xpdl:pivotTableDefinition16/>
-    </ext>
-  </extLst>
-</pivotTableDefinition>
-</file>
-
-<file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable6" cacheId="6" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="7" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="7" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="9" rowHeaderCaption="Region">
-  <location ref="J12:K16" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
-  <pivotFields count="9">
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField dataField="1" showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0">
-      <items count="14">
-        <item x="0"/>
-        <item x="1"/>
-        <item x="2"/>
-        <item x="3"/>
-        <item x="4"/>
-        <item x="5"/>
-        <item x="6"/>
-        <item x="7"/>
-        <item x="8"/>
-        <item x="9"/>
-        <item x="10"/>
-        <item x="11"/>
-        <item x="12"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField axis="axisRow" showAll="0">
-      <items count="4">
-        <item sd="0" x="1"/>
-        <item sd="0" x="2"/>
-        <item sd="0" x="0"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-  </pivotFields>
-  <rowFields count="1">
-    <field x="8"/>
-  </rowFields>
-  <rowItems count="4">
-    <i>
-      <x/>
-    </i>
-    <i>
-      <x v="1"/>
-    </i>
-    <i>
-      <x v="2"/>
-    </i>
-    <i t="grand">
-      <x/>
-    </i>
-  </rowItems>
-  <colItems count="1">
-    <i/>
-  </colItems>
-  <dataFields count="1">
-    <dataField name="Min of Cylinders" fld="2" subtotal="min" baseField="8" baseItem="0"/>
-  </dataFields>
-  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
-      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
-    </ext>
-    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
-      <xpdl:pivotTableDefinition16/>
-    </ext>
-  </extLst>
-</pivotTableDefinition>
-</file>
-
-<file path=xl/pivotTables/pivotTable3.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable5" cacheId="6" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="7" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="7" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="9" rowHeaderCaption="Region">
-  <location ref="G12:H16" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
-  <pivotFields count="9">
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField dataField="1" showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0">
-      <items count="14">
-        <item x="0"/>
-        <item x="1"/>
-        <item x="2"/>
-        <item x="3"/>
-        <item x="4"/>
-        <item x="5"/>
-        <item x="6"/>
-        <item x="7"/>
-        <item x="8"/>
-        <item x="9"/>
-        <item x="10"/>
-        <item x="11"/>
-        <item x="12"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField axis="axisRow" showAll="0">
-      <items count="4">
-        <item sd="0" x="1"/>
-        <item sd="0" x="2"/>
-        <item sd="0" x="0"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-  </pivotFields>
-  <rowFields count="1">
-    <field x="8"/>
-  </rowFields>
-  <rowItems count="4">
-    <i>
-      <x/>
-    </i>
-    <i>
-      <x v="1"/>
-    </i>
-    <i>
-      <x v="2"/>
-    </i>
-    <i t="grand">
-      <x/>
-    </i>
-  </rowItems>
-  <colItems count="1">
-    <i/>
-  </colItems>
-  <dataFields count="1">
-    <dataField name="Max of Cylinders" fld="2" subtotal="max" baseField="8" baseItem="0"/>
-  </dataFields>
-  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
-      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
-    </ext>
-    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
-      <xpdl:pivotTableDefinition16/>
-    </ext>
-  </extLst>
-</pivotTableDefinition>
-</file>
-
-<file path=xl/pivotTables/pivotTable4.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable4" cacheId="6" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="7" minRefreshableVersion="3" useAutoFormatting="1" rowGrandTotals="0" colGrandTotals="0" itemPrintTitles="1" createdVersion="7" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="9" rowHeaderCaption="Region">
-  <location ref="K3:L6" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
-  <pivotFields count="9">
-    <pivotField showAll="0"/>
-    <pivotField dataField="1" showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0">
-      <items count="14">
-        <item x="0"/>
-        <item x="1"/>
-        <item x="2"/>
-        <item x="3"/>
-        <item x="4"/>
-        <item x="5"/>
-        <item x="6"/>
-        <item x="7"/>
-        <item x="8"/>
-        <item x="9"/>
-        <item x="10"/>
-        <item x="11"/>
-        <item x="12"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField axis="axisRow" showAll="0">
-      <items count="4">
-        <item sd="0" x="1"/>
-        <item sd="0" x="2"/>
-        <item sd="0" x="0"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-  </pivotFields>
-  <rowFields count="1">
-    <field x="8"/>
-  </rowFields>
-  <rowItems count="3">
-    <i>
-      <x/>
-    </i>
-    <i>
-      <x v="1"/>
-    </i>
-    <i>
-      <x v="2"/>
-    </i>
-  </rowItems>
-  <colItems count="1">
-    <i/>
-  </colItems>
-  <dataFields count="1">
-    <dataField name="Average of MPG" fld="1" subtotal="average" baseField="8" baseItem="0"/>
-  </dataFields>
-  <chartFormats count="4">
-    <chartFormat chart="8" format="5" series="1">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="1">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="8" format="6">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="2">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-          <reference field="8" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="8" format="7">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="2">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-          <reference field="8" count="1" selected="0">
-            <x v="1"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="8" format="8">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="2">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-          <reference field="8" count="1" selected="0">
-            <x v="2"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-  </chartFormats>
-  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
-      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
-    </ext>
-    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
-      <xpdl:pivotTableDefinition16/>
-    </ext>
-  </extLst>
-</pivotTableDefinition>
-</file>
-
-<file path=xl/pivotTables/pivotTable5.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable3" cacheId="6" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="7" minRefreshableVersion="3" useAutoFormatting="1" rowGrandTotals="0" colGrandTotals="0" itemPrintTitles="1" createdVersion="7" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="6" rowHeaderCaption="Region">
-  <location ref="G3:H6" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
-  <pivotFields count="9">
-    <pivotField dataField="1" showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0">
-      <items count="14">
-        <item x="0"/>
-        <item x="1"/>
-        <item x="2"/>
-        <item x="3"/>
-        <item x="4"/>
-        <item x="5"/>
-        <item x="6"/>
-        <item x="7"/>
-        <item x="8"/>
-        <item x="9"/>
-        <item x="10"/>
-        <item x="11"/>
-        <item x="12"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField axis="axisRow" showAll="0">
-      <items count="4">
-        <item sd="0" x="1"/>
-        <item sd="0" x="2"/>
-        <item sd="0" x="0"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-  </pivotFields>
-  <rowFields count="1">
-    <field x="8"/>
-  </rowFields>
-  <rowItems count="3">
-    <i>
-      <x/>
-    </i>
-    <i>
-      <x v="1"/>
-    </i>
-    <i>
-      <x v="2"/>
-    </i>
-  </rowItems>
-  <colItems count="1">
-    <i/>
-  </colItems>
-  <dataFields count="1">
-    <dataField name="Count of Car" fld="0" subtotal="count" baseField="0" baseItem="0"/>
-  </dataFields>
-  <chartFormats count="1">
-    <chartFormat chart="5" format="2" series="1">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="1">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-  </chartFormats>
-  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
-      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
-    </ext>
-    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
-      <xpdl:pivotTableDefinition16/>
-    </ext>
-  </extLst>
-</pivotTableDefinition>
-</file>
-
-<file path=xl/pivotTables/pivotTable6.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable2" cacheId="6" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="7" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="7" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="3" rowHeaderCaption="Model">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00000000-0007-0000-0100-000000000000}" name="PivotTable2" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="7" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="7" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="3" rowHeaderCaption="Model">
   <location ref="A3:B17" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="9">
     <pivotField dataField="1" showAll="0"/>
@@ -10379,8 +9874,8 @@
     <pivotField showAll="0">
       <items count="4">
         <item sd="0" x="1"/>
-        <item sd="0" x="2"/>
-        <item sd="0" x="0"/>
+        <item h="1" sd="0" x="2"/>
+        <item h="1" sd="0" x="0"/>
         <item t="default"/>
       </items>
     </pivotField>
@@ -10461,8 +9956,401 @@
 </pivotTableDefinition>
 </file>
 
+<file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00000000-0007-0000-0100-000005000000}" name="PivotTable7" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="7" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="7" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="9" rowHeaderCaption="Region">
+  <location ref="A21:B23" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
+  <pivotFields count="9">
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField dataField="1" showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0">
+      <items count="14">
+        <item x="0"/>
+        <item x="1"/>
+        <item x="2"/>
+        <item x="3"/>
+        <item x="4"/>
+        <item x="5"/>
+        <item x="6"/>
+        <item x="7"/>
+        <item x="8"/>
+        <item x="9"/>
+        <item x="10"/>
+        <item x="11"/>
+        <item x="12"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField axis="axisRow" showAll="0">
+      <items count="4">
+        <item sd="0" x="1"/>
+        <item h="1" sd="0" x="2"/>
+        <item h="1" sd="0" x="0"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+  </pivotFields>
+  <rowFields count="1">
+    <field x="8"/>
+  </rowFields>
+  <rowItems count="2">
+    <i>
+      <x/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </rowItems>
+  <colItems count="1">
+    <i/>
+  </colItems>
+  <dataFields count="1">
+    <dataField name="Average of Horsepower" fld="4" subtotal="average" baseField="8" baseItem="0"/>
+  </dataFields>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
+      <xpdl:pivotTableDefinition16/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
+<file path=xl/pivotTables/pivotTable3.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00000000-0007-0000-0100-000004000000}" name="PivotTable6" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="7" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="7" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="9" rowHeaderCaption="Region">
+  <location ref="J12:K14" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
+  <pivotFields count="9">
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField dataField="1" showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0">
+      <items count="14">
+        <item x="0"/>
+        <item x="1"/>
+        <item x="2"/>
+        <item x="3"/>
+        <item x="4"/>
+        <item x="5"/>
+        <item x="6"/>
+        <item x="7"/>
+        <item x="8"/>
+        <item x="9"/>
+        <item x="10"/>
+        <item x="11"/>
+        <item x="12"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField axis="axisRow" showAll="0">
+      <items count="4">
+        <item sd="0" x="1"/>
+        <item h="1" sd="0" x="2"/>
+        <item h="1" sd="0" x="0"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+  </pivotFields>
+  <rowFields count="1">
+    <field x="8"/>
+  </rowFields>
+  <rowItems count="2">
+    <i>
+      <x/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </rowItems>
+  <colItems count="1">
+    <i/>
+  </colItems>
+  <dataFields count="1">
+    <dataField name="Min of Cylinders" fld="2" subtotal="min" baseField="8" baseItem="0"/>
+  </dataFields>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
+      <xpdl:pivotTableDefinition16/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
+<file path=xl/pivotTables/pivotTable4.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00000000-0007-0000-0100-000003000000}" name="PivotTable5" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="7" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="7" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="9" rowHeaderCaption="Region">
+  <location ref="G12:H14" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
+  <pivotFields count="9">
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField dataField="1" showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0">
+      <items count="14">
+        <item x="0"/>
+        <item x="1"/>
+        <item x="2"/>
+        <item x="3"/>
+        <item x="4"/>
+        <item x="5"/>
+        <item x="6"/>
+        <item x="7"/>
+        <item x="8"/>
+        <item x="9"/>
+        <item x="10"/>
+        <item x="11"/>
+        <item x="12"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField axis="axisRow" showAll="0">
+      <items count="4">
+        <item sd="0" x="1"/>
+        <item h="1" sd="0" x="2"/>
+        <item h="1" sd="0" x="0"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+  </pivotFields>
+  <rowFields count="1">
+    <field x="8"/>
+  </rowFields>
+  <rowItems count="2">
+    <i>
+      <x/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </rowItems>
+  <colItems count="1">
+    <i/>
+  </colItems>
+  <dataFields count="1">
+    <dataField name="Max of Cylinders" fld="2" subtotal="max" baseField="8" baseItem="0"/>
+  </dataFields>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
+      <xpdl:pivotTableDefinition16/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
+<file path=xl/pivotTables/pivotTable5.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00000000-0007-0000-0100-000002000000}" name="PivotTable4" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="7" minRefreshableVersion="3" useAutoFormatting="1" rowGrandTotals="0" colGrandTotals="0" itemPrintTitles="1" createdVersion="7" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="9" rowHeaderCaption="Region">
+  <location ref="K3:L4" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
+  <pivotFields count="9">
+    <pivotField showAll="0"/>
+    <pivotField dataField="1" showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0">
+      <items count="14">
+        <item x="0"/>
+        <item x="1"/>
+        <item x="2"/>
+        <item x="3"/>
+        <item x="4"/>
+        <item x="5"/>
+        <item x="6"/>
+        <item x="7"/>
+        <item x="8"/>
+        <item x="9"/>
+        <item x="10"/>
+        <item x="11"/>
+        <item x="12"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField axis="axisRow" showAll="0">
+      <items count="4">
+        <item sd="0" x="1"/>
+        <item h="1" sd="0" x="2"/>
+        <item h="1" sd="0" x="0"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+  </pivotFields>
+  <rowFields count="1">
+    <field x="8"/>
+  </rowFields>
+  <rowItems count="1">
+    <i>
+      <x/>
+    </i>
+  </rowItems>
+  <colItems count="1">
+    <i/>
+  </colItems>
+  <dataFields count="1">
+    <dataField name="Average of MPG" fld="1" subtotal="average" baseField="8" baseItem="0"/>
+  </dataFields>
+  <chartFormats count="4">
+    <chartFormat chart="8" format="5" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="8" format="6">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="8" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="8" format="7">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="8" count="1" selected="0">
+            <x v="1"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="8" format="8">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="8" count="1" selected="0">
+            <x v="2"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+  </chartFormats>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
+      <xpdl:pivotTableDefinition16/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
+<file path=xl/pivotTables/pivotTable6.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00000000-0007-0000-0100-000001000000}" name="PivotTable3" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="7" minRefreshableVersion="3" useAutoFormatting="1" rowGrandTotals="0" colGrandTotals="0" itemPrintTitles="1" createdVersion="7" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="6" rowHeaderCaption="Region">
+  <location ref="G3:H6" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
+  <pivotFields count="9">
+    <pivotField dataField="1" showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0">
+      <items count="14">
+        <item x="0"/>
+        <item x="1"/>
+        <item x="2"/>
+        <item x="3"/>
+        <item x="4"/>
+        <item x="5"/>
+        <item x="6"/>
+        <item x="7"/>
+        <item x="8"/>
+        <item x="9"/>
+        <item x="10"/>
+        <item x="11"/>
+        <item x="12"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField axis="axisRow" showAll="0">
+      <items count="4">
+        <item sd="0" x="1"/>
+        <item sd="0" x="2"/>
+        <item sd="0" x="0"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+  </pivotFields>
+  <rowFields count="1">
+    <field x="8"/>
+  </rowFields>
+  <rowItems count="3">
+    <i>
+      <x/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="2"/>
+    </i>
+  </rowItems>
+  <colItems count="1">
+    <i/>
+  </colItems>
+  <dataFields count="1">
+    <dataField name="Count of Car" fld="0" subtotal="count" baseField="0" baseItem="0"/>
+  </dataFields>
+  <chartFormats count="1">
+    <chartFormat chart="5" format="2" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+  </chartFormats>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
+      <xpdl:pivotTableDefinition16/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
 <file path=xl/queryTables/queryTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="ExternalData_1" connectionId="1" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0">
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="ExternalData_1" connectionId="1" xr16:uid="{00000000-0016-0000-0000-000000000000}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0">
   <queryTableRefresh nextId="10">
     <queryTableFields count="9">
       <queryTableField id="1" name="Car" tableColumnId="1"/>
@@ -10480,7 +10368,7 @@
 </file>
 
 <file path=xl/slicerCaches/slicerCache1.xml><?xml version="1.0" encoding="utf-8"?>
-<slicerCacheDefinition xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" mc:Ignorable="x" name="Slicer_Origin" sourceName="Origin">
+<slicerCacheDefinition xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x xr10" name="Slicer_Origin" xr10:uid="{00000000-0013-0000-FFFF-FFFF01000000}" sourceName="Origin">
   <pivotTables>
     <pivotTable tabId="4" name="PivotTable2"/>
     <pivotTable tabId="4" name="PivotTable4"/>
@@ -10492,8 +10380,8 @@
     <tabular pivotCacheId="1991815873" customListSort="0">
       <items count="3">
         <i x="1" s="1"/>
-        <i x="2" s="1"/>
-        <i x="0" s="1"/>
+        <i x="2"/>
+        <i x="0"/>
       </items>
     </tabular>
   </data>
@@ -10501,24 +10389,24 @@
 </file>
 
 <file path=xl/slicers/slicer1.xml><?xml version="1.0" encoding="utf-8"?>
-<slicers xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" mc:Ignorable="x">
-  <slicer name="Origin" cache="Slicer_Origin" caption="Origin" columnCount="3" showCaption="0" style="SlicerStyleLight5" rowHeight="241300"/>
+<slicers xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x xr10">
+  <slicer name="Origin" xr10:uid="{00000000-0014-0000-FFFF-FFFF01000000}" cache="Slicer_Origin" caption="Origin" columnCount="3" showCaption="0" style="SlicerStyleLight5" rowHeight="241300"/>
 </slicers>
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Cars" displayName="Cars" ref="A1:I407" tableType="queryTable" totalsRowShown="0">
-  <autoFilter ref="A1:I407"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Cars" displayName="Cars" ref="A1:I407" tableType="queryTable" totalsRowShown="0">
+  <autoFilter ref="A1:I407" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <tableColumns count="9">
-    <tableColumn id="1" uniqueName="1" name="Car" queryTableFieldId="1" dataDxfId="1"/>
-    <tableColumn id="2" uniqueName="2" name="MPG" queryTableFieldId="2"/>
-    <tableColumn id="3" uniqueName="3" name="Cylinders" queryTableFieldId="3"/>
-    <tableColumn id="4" uniqueName="4" name="Displacement" queryTableFieldId="4"/>
-    <tableColumn id="5" uniqueName="5" name="Horsepower" queryTableFieldId="5"/>
-    <tableColumn id="6" uniqueName="6" name="Weight" queryTableFieldId="6"/>
-    <tableColumn id="7" uniqueName="7" name="Acceleration" queryTableFieldId="7"/>
-    <tableColumn id="8" uniqueName="8" name="Model" queryTableFieldId="8"/>
-    <tableColumn id="9" uniqueName="9" name="Origin" queryTableFieldId="9" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" uniqueName="1" name="Car" queryTableFieldId="1" dataDxfId="1"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" uniqueName="2" name="MPG" queryTableFieldId="2"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" uniqueName="3" name="Cylinders" queryTableFieldId="3"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" uniqueName="4" name="Displacement" queryTableFieldId="4"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" uniqueName="5" name="Horsepower" queryTableFieldId="5"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" uniqueName="6" name="Weight" queryTableFieldId="6"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" uniqueName="7" name="Acceleration" queryTableFieldId="7"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" uniqueName="8" name="Model" queryTableFieldId="8"/>
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" uniqueName="9" name="Origin" queryTableFieldId="9" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -10820,7 +10708,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I407"/>
   <sheetViews>
     <sheetView showGridLines="0" topLeftCell="A2" workbookViewId="0">
@@ -22651,8 +22539,8 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A3:L25"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A3:L23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="J18" sqref="J18"/>
@@ -22694,7 +22582,7 @@
         <v>70</v>
       </c>
       <c r="B4" s="1">
-        <v>35</v>
+        <v>6</v>
       </c>
       <c r="G4" s="3" t="s">
         <v>21</v>
@@ -22714,19 +22602,13 @@
         <v>71</v>
       </c>
       <c r="B5" s="1">
-        <v>29</v>
+        <v>5</v>
       </c>
       <c r="G5" s="3" t="s">
         <v>32</v>
       </c>
       <c r="H5" s="1">
         <v>79</v>
-      </c>
-      <c r="K5" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="L5" s="1">
-        <v>304.50632911392404</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
@@ -22734,19 +22616,13 @@
         <v>72</v>
       </c>
       <c r="B6" s="1">
-        <v>28</v>
+        <v>5</v>
       </c>
       <c r="G6" s="3" t="s">
         <v>10</v>
       </c>
       <c r="H6" s="1">
         <v>254</v>
-      </c>
-      <c r="K6" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="L6" s="1">
-        <v>196.88188976377953</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
@@ -22754,7 +22630,7 @@
         <v>73</v>
       </c>
       <c r="B7" s="1">
-        <v>40</v>
+        <v>7</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
@@ -22762,7 +22638,7 @@
         <v>74</v>
       </c>
       <c r="B8" s="1">
-        <v>27</v>
+        <v>6</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
@@ -22770,7 +22646,7 @@
         <v>75</v>
       </c>
       <c r="B9" s="1">
-        <v>30</v>
+        <v>6</v>
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
@@ -22778,7 +22654,7 @@
         <v>76</v>
       </c>
       <c r="B10" s="1">
-        <v>34</v>
+        <v>8</v>
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
@@ -22786,7 +22662,7 @@
         <v>77</v>
       </c>
       <c r="B11" s="1">
-        <v>28</v>
+        <v>4</v>
       </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
@@ -22794,7 +22670,7 @@
         <v>78</v>
       </c>
       <c r="B12" s="1">
-        <v>36</v>
+        <v>6</v>
       </c>
       <c r="G12" s="2" t="s">
         <v>325</v>
@@ -22814,7 +22690,7 @@
         <v>79</v>
       </c>
       <c r="B13" s="1">
-        <v>29</v>
+        <v>4</v>
       </c>
       <c r="G13" s="3" t="s">
         <v>21</v>
@@ -22834,19 +22710,19 @@
         <v>80</v>
       </c>
       <c r="B14" s="1">
-        <v>29</v>
+        <v>9</v>
       </c>
       <c r="G14" s="3" t="s">
-        <v>32</v>
+        <v>320</v>
       </c>
       <c r="H14" s="1">
         <v>6</v>
       </c>
       <c r="J14" s="3" t="s">
-        <v>32</v>
+        <v>320</v>
       </c>
       <c r="K14" s="1">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.25">
@@ -22854,19 +22730,7 @@
         <v>81</v>
       </c>
       <c r="B15" s="1">
-        <v>30</v>
-      </c>
-      <c r="G15" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="H15" s="1">
-        <v>8</v>
-      </c>
-      <c r="J15" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="K15" s="1">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.25">
@@ -22874,19 +22738,7 @@
         <v>82</v>
       </c>
       <c r="B16" s="1">
-        <v>31</v>
-      </c>
-      <c r="G16" s="3" t="s">
-        <v>320</v>
-      </c>
-      <c r="H16" s="1">
-        <v>8</v>
-      </c>
-      <c r="J16" s="3" t="s">
-        <v>320</v>
-      </c>
-      <c r="K16" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
@@ -22894,7 +22746,7 @@
         <v>320</v>
       </c>
       <c r="B17" s="1">
-        <v>406</v>
+        <v>73</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
@@ -22915,26 +22767,10 @@
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="s">
-        <v>32</v>
+        <v>320</v>
       </c>
       <c r="B23" s="1">
-        <v>6949.1139240506327</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A24" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="B24" s="1">
-        <v>4060.1181102362207</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A25" s="3" t="s">
-        <v>320</v>
-      </c>
-      <c r="B25" s="1">
-        <v>4955.1724137931033</v>
+        <v>5911.6438356164381</v>
       </c>
     </row>
   </sheetData>
@@ -22943,11 +22779,11 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="B1:L11"/>
   <sheetViews>
     <sheetView showGridLines="0" showRowColHeaders="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+      <selection activeCell="I10" sqref="I10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -22966,143 +22802,143 @@
     <col min="13" max="16384" width="9.140625" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:12" s="12" customFormat="1" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C1" s="17"/>
-      <c r="D1" s="15" t="s">
+    <row r="1" spans="2:12" s="6" customFormat="1" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C1" s="9"/>
+      <c r="D1" s="12" t="s">
         <v>331</v>
       </c>
-      <c r="E1" s="15"/>
-      <c r="F1" s="15"/>
-      <c r="G1" s="15"/>
-      <c r="H1" s="15"/>
-      <c r="I1" s="15"/>
-      <c r="J1" s="15"/>
-      <c r="K1" s="15"/>
-      <c r="L1" s="15"/>
-    </row>
-    <row r="2" spans="2:12" s="13" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="14"/>
-      <c r="C2" s="14"/>
-      <c r="D2" s="19"/>
-      <c r="E2" s="19"/>
-      <c r="F2" s="19"/>
-      <c r="G2" s="19"/>
-      <c r="H2" s="19"/>
-      <c r="I2" s="19"/>
-      <c r="J2" s="19"/>
-      <c r="K2" s="19"/>
-      <c r="L2" s="19"/>
-    </row>
-    <row r="3" spans="2:12" s="13" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="14"/>
-      <c r="C3" s="14"/>
-      <c r="D3" s="19"/>
-      <c r="E3" s="19"/>
-      <c r="F3" s="19"/>
-      <c r="G3" s="19"/>
-      <c r="H3" s="19"/>
-      <c r="I3" s="19"/>
-      <c r="J3" s="19"/>
-      <c r="K3" s="19"/>
-      <c r="L3" s="19"/>
-    </row>
-    <row r="4" spans="2:12" s="13" customFormat="1" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="18"/>
-      <c r="C4" s="18"/>
-      <c r="D4" s="16"/>
-      <c r="E4" s="16"/>
-      <c r="F4" s="16"/>
-      <c r="G4" s="16"/>
-      <c r="H4" s="16"/>
-      <c r="I4" s="16"/>
-      <c r="J4" s="16"/>
-      <c r="K4" s="16"/>
-      <c r="L4" s="16"/>
+      <c r="E1" s="12"/>
+      <c r="F1" s="12"/>
+      <c r="G1" s="12"/>
+      <c r="H1" s="12"/>
+      <c r="I1" s="12"/>
+      <c r="J1" s="12"/>
+      <c r="K1" s="12"/>
+      <c r="L1" s="12"/>
+    </row>
+    <row r="2" spans="2:12" s="7" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B2" s="8"/>
+      <c r="C2" s="8"/>
+      <c r="D2" s="13"/>
+      <c r="E2" s="13"/>
+      <c r="F2" s="13"/>
+      <c r="G2" s="13"/>
+      <c r="H2" s="13"/>
+      <c r="I2" s="13"/>
+      <c r="J2" s="13"/>
+      <c r="K2" s="13"/>
+      <c r="L2" s="13"/>
+    </row>
+    <row r="3" spans="2:12" s="7" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B3" s="8"/>
+      <c r="C3" s="8"/>
+      <c r="D3" s="13"/>
+      <c r="E3" s="13"/>
+      <c r="F3" s="13"/>
+      <c r="G3" s="13"/>
+      <c r="H3" s="13"/>
+      <c r="I3" s="13"/>
+      <c r="J3" s="13"/>
+      <c r="K3" s="13"/>
+      <c r="L3" s="13"/>
+    </row>
+    <row r="4" spans="2:12" s="7" customFormat="1" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B4" s="10"/>
+      <c r="C4" s="10"/>
+      <c r="D4" s="14"/>
+      <c r="E4" s="14"/>
+      <c r="F4" s="14"/>
+      <c r="G4" s="14"/>
+      <c r="H4" s="14"/>
+      <c r="I4" s="14"/>
+      <c r="J4" s="14"/>
+      <c r="K4" s="14"/>
+      <c r="L4" s="14"/>
     </row>
     <row r="5" spans="2:12" s="4" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="6" spans="2:12" ht="26.25" x14ac:dyDescent="0.25">
-      <c r="B6" s="6" t="s">
+      <c r="B6" s="15" t="s">
         <v>327</v>
       </c>
-      <c r="C6" s="7"/>
-      <c r="E6" s="6" t="s">
+      <c r="C6" s="16"/>
+      <c r="E6" s="15" t="s">
         <v>328</v>
       </c>
-      <c r="F6" s="7"/>
-      <c r="H6" s="6" t="s">
+      <c r="F6" s="16"/>
+      <c r="H6" s="15" t="s">
         <v>329</v>
       </c>
-      <c r="I6" s="7"/>
-      <c r="K6" s="6" t="s">
+      <c r="I6" s="16"/>
+      <c r="K6" s="15" t="s">
         <v>330</v>
       </c>
-      <c r="L6" s="7"/>
+      <c r="L6" s="16"/>
     </row>
     <row r="7" spans="2:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="8">
+      <c r="B7" s="17">
         <f>GETPIVOTDATA("Car",Calculations!$A$3)</f>
-        <v>406</v>
-      </c>
-      <c r="C7" s="9"/>
-      <c r="E7" s="8">
+        <v>73</v>
+      </c>
+      <c r="C7" s="18"/>
+      <c r="E7" s="17">
         <f>GETPIVOTDATA("Cylinders",Calculations!$J$12)</f>
-        <v>3</v>
-      </c>
-      <c r="F7" s="9"/>
-      <c r="H7" s="8">
+        <v>4</v>
+      </c>
+      <c r="F7" s="18"/>
+      <c r="H7" s="17">
         <f>GETPIVOTDATA("Cylinders",Calculations!$G$12)</f>
-        <v>8</v>
-      </c>
-      <c r="I7" s="9"/>
-      <c r="K7" s="8">
+        <v>6</v>
+      </c>
+      <c r="I7" s="18"/>
+      <c r="K7" s="17">
         <f>GETPIVOTDATA("Horsepower",Calculations!$A$21)</f>
-        <v>4955.1724137931033</v>
-      </c>
-      <c r="L7" s="9"/>
+        <v>5911.6438356164381</v>
+      </c>
+      <c r="L7" s="18"/>
     </row>
     <row r="8" spans="2:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="10"/>
-      <c r="C8" s="11"/>
-      <c r="E8" s="10"/>
-      <c r="F8" s="11"/>
-      <c r="H8" s="10"/>
-      <c r="I8" s="11"/>
-      <c r="K8" s="10"/>
-      <c r="L8" s="11"/>
+      <c r="B8" s="19"/>
+      <c r="C8" s="20"/>
+      <c r="E8" s="19"/>
+      <c r="F8" s="20"/>
+      <c r="H8" s="19"/>
+      <c r="I8" s="20"/>
+      <c r="K8" s="19"/>
+      <c r="L8" s="20"/>
     </row>
     <row r="9" spans="2:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="21"/>
-      <c r="C9" s="21"/>
-      <c r="E9" s="21"/>
-      <c r="F9" s="21"/>
-      <c r="H9" s="21"/>
-      <c r="I9" s="21"/>
-      <c r="K9" s="20"/>
-      <c r="L9" s="20"/>
+      <c r="B9" s="11"/>
+      <c r="C9" s="11"/>
+      <c r="E9" s="11"/>
+      <c r="F9" s="11"/>
+      <c r="H9" s="11"/>
+      <c r="I9" s="11"/>
+      <c r="K9" s="21"/>
+      <c r="L9" s="21"/>
     </row>
     <row r="10" spans="2:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="21"/>
-      <c r="C10" s="21"/>
-      <c r="E10" s="21"/>
-      <c r="F10" s="21"/>
-      <c r="H10" s="21"/>
-      <c r="I10" s="21"/>
-      <c r="K10" s="21"/>
-      <c r="L10" s="21"/>
+      <c r="B10" s="11"/>
+      <c r="C10" s="11"/>
+      <c r="E10" s="11"/>
+      <c r="F10" s="11"/>
+      <c r="H10" s="11"/>
+      <c r="I10" s="11"/>
+      <c r="K10" s="11"/>
+      <c r="L10" s="11"/>
     </row>
     <row r="11" spans="2:12" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="K7:L8"/>
+    <mergeCell ref="K9:L9"/>
+    <mergeCell ref="H7:I8"/>
+    <mergeCell ref="B7:C8"/>
+    <mergeCell ref="E7:F8"/>
     <mergeCell ref="D1:L4"/>
     <mergeCell ref="B6:C6"/>
     <mergeCell ref="K6:L6"/>
     <mergeCell ref="H6:I6"/>
     <mergeCell ref="E6:F6"/>
-    <mergeCell ref="K7:L8"/>
-    <mergeCell ref="K9:L9"/>
-    <mergeCell ref="H7:I8"/>
-    <mergeCell ref="B7:C8"/>
-    <mergeCell ref="E7:F8"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>